<commit_message>
practice handsOn: jsonPlaceholder post curd app added
</commit_message>
<xml_diff>
--- a/Session_Plan.xlsx
+++ b/Session_Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>React 6-Day Learning Plan Time Breakdown</t>
   </si>
@@ -35,27 +35,18 @@
     <t>Topics</t>
   </si>
   <si>
-    <t>Estimated Time</t>
-  </si>
-  <si>
     <t>Day 1</t>
   </si>
   <si>
     <t>React Fundamentals, JSX, Components, Props</t>
   </si>
   <si>
-    <t>3–4 hrs</t>
-  </si>
-  <si>
     <t>Day 2</t>
   </si>
   <si>
     <t>Day 3</t>
   </si>
   <si>
-    <t>2.5–3.5 hrs</t>
-  </si>
-  <si>
     <t>Day 4</t>
   </si>
   <si>
@@ -68,16 +59,10 @@
     <t>Context API, Prop Drilling, Custom Hooks</t>
   </si>
   <si>
-    <t>2.5–3 hrs</t>
-  </si>
-  <si>
     <t>Day 6</t>
   </si>
   <si>
     <t>React Router, Final Mini Project</t>
-  </si>
-  <si>
-    <t>4–5 hrs</t>
   </si>
   <si>
     <t>useState, Events, Lists, Conditional Render</t>
@@ -151,9 +136,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -163,12 +145,15 @@
     <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <font>
         <strike val="0"/>
@@ -182,20 +167,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -267,12 +238,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A3:D9"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Day" dataDxfId="3"/>
-    <tableColumn id="2" name="Topics" dataDxfId="2"/>
-    <tableColumn id="3" name="Estimated Time" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:C9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A3:C9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Day" dataDxfId="2"/>
+    <tableColumn id="2" name="Topics" dataDxfId="1"/>
     <tableColumn id="4" name="Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -542,124 +512,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
-        <v>45754</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45755</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4">
-        <v>45756</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C8" s="3">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4">
-        <v>45757</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4">
-        <v>45758</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4">
-        <v>45759</v>
+      <c r="C9" s="3">
+        <v>45787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>